<commit_message>
update model to latest version of sisepuede
</commit_message>
<xml_diff>
--- a/ssp_modeling/scenario_mapping/ssp_egypt_transformation_cw.xlsx
+++ b/ssp_modeling/scenario_mapping/ssp_egypt_transformation_cw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tony/Documents/sisepuede_modeling/ssp_egypt/ssp_modeling/scenario_mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFED887-37DA-C64F-B701-EF87DB2ACD80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0992AD1-8568-A648-AC02-91DA757AC63F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4080" yWindow="500" windowWidth="30240" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -1919,7 +1919,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>